<commit_message>
remove unnecessary lines from codes
</commit_message>
<xml_diff>
--- a/public/attendance.xlsx
+++ b/public/attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhrvr\Desktop\Staff mgt\STAFF_MGT_SYS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D723EB2-3D1E-4BD3-A25B-F3EECBDA9E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CB5E60-66FC-464A-BF6E-A11B2A266CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0E15837C-5C5B-4AA0-A15A-66ACAE137DD5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>11:00AM</t>
+  </si>
+  <si>
+    <t>Deep Javya</t>
+  </si>
+  <si>
+    <t>08:59AM</t>
   </si>
 </sst>
 </file>
@@ -109,7 +115,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-14009]dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -215,7 +221,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -552,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8D5C66-DAF3-4118-A545-9282C104B3D2}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A2:A6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,6 +688,23 @@
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
     </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9">
+        <v>45408</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>